<commit_message>
feat : ResourceNode 수정
</commit_message>
<xml_diff>
--- a/Monster_Info.xlsx
+++ b/Monster_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alama\Documents\GitHub\DungeonRPGDataFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\2_UNITIYGAME\DungeonRPG\Assets\JJData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFC0688-F52C-4C8A-85D0-5ED4FC4C24DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65B8920-6854-4895-A52C-7F071B8C1C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="1" r:id="rId1"/>
@@ -586,24 +586,25 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="Item"/>
       <sheetName val="UseItem"/>
       <sheetName val="DropItem"/>
+      <sheetName val="Weapon"/>
+      <sheetName val="Armor"/>
+      <sheetName val="Backpack"/>
+      <sheetName val="Pouch"/>
       <sheetName val="Potion"/>
-      <sheetName val="Tool"/>
-      <sheetName val="Armor"/>
       <sheetName val="ResourceNode"/>
       <sheetName val="ResourceNode_DropTable"/>
       <sheetName val="Condition"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
         <row r="1">
           <cell r="B1" t="str">
             <v>아이템 id</v>
@@ -616,51 +617,23 @@
         </row>
         <row r="3">
           <cell r="B3" t="str">
-            <v>Item_id</v>
+            <v>UseItem_id</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4" t="str">
-            <v>ITM_DRP_001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>ITM_HER_JSM</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>ITM_HER_JNB</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>ITM_HER_RSM</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>ITM_MIN_CPR</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>ITM_MIN_SIL</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>ITM_MIN_GOL</v>
+            <v>PAR_DRP_SCR</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1208,7 +1181,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1525,7 +1498,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1605,7 +1578,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>